<commit_message>
Updated with new data and new regression model
</commit_message>
<xml_diff>
--- a/BT2101 Survey  (Responses).xlsx
+++ b/BT2101 Survey  (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="56">
   <si>
     <t>Timestamp</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>6-12 months</t>
+  </si>
+  <si>
+    <t>Na</t>
   </si>
 </sst>
 </file>
@@ -640,7 +643,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:AA45" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:AA53" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="27">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="What is your age?" id="2"/>
@@ -4369,80 +4372,702 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="24">
+      <c r="A45" s="17">
         <v>45742.42840638889</v>
       </c>
-      <c r="B45" s="25">
+      <c r="B45" s="18">
         <v>20.0</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="25">
+      <c r="F45" s="18">
         <v>45.0</v>
       </c>
-      <c r="G45" s="25" t="s">
+      <c r="G45" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H45" s="25" t="s">
+      <c r="H45" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I45" s="25">
+      <c r="I45" s="18">
         <v>4.23</v>
       </c>
-      <c r="J45" s="25">
+      <c r="J45" s="18">
         <v>4.44</v>
       </c>
-      <c r="K45" s="25" t="s">
+      <c r="K45" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L45" s="25" t="s">
+      <c r="L45" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M45" s="25" t="s">
+      <c r="M45" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="N45" s="25">
-        <v>4.0</v>
-      </c>
-      <c r="O45" s="25">
-        <v>2.0</v>
-      </c>
-      <c r="P45" s="25">
-        <v>3.0</v>
-      </c>
-      <c r="Q45" s="25">
-        <v>4.0</v>
-      </c>
-      <c r="R45" s="25">
-        <v>4.0</v>
-      </c>
-      <c r="S45" s="25">
-        <v>3.0</v>
-      </c>
-      <c r="T45" s="25">
-        <v>4.0</v>
-      </c>
-      <c r="U45" s="25" t="s">
+      <c r="N45" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="O45" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="P45" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Q45" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="R45" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="S45" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="T45" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="U45" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="V45" s="25">
-        <v>4.0</v>
-      </c>
-      <c r="W45" s="25">
-        <v>3.0</v>
-      </c>
-      <c r="X45" s="25">
-        <v>3.0</v>
-      </c>
-      <c r="Y45" s="25">
-        <v>3.0</v>
-      </c>
-      <c r="Z45" s="25">
-        <v>3.0</v>
-      </c>
-      <c r="AA45" s="26">
-        <v>4.0</v>
+      <c r="V45" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="W45" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="X45" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Y45" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Z45" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="AA45" s="19">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="14">
+        <v>45742.44317925926</v>
+      </c>
+      <c r="B46" s="15">
+        <v>20.0</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="15">
+        <v>85.0</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I46" s="15">
+        <v>4.2</v>
+      </c>
+      <c r="J46" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L46" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M46" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="O46" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="P46" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="Q46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="R46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="S46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="T46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="U46" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="V46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="W46" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="X46" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="Y46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="Z46" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="AA46" s="16">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="17">
+        <v>45742.4445903125</v>
+      </c>
+      <c r="B47" s="18">
+        <v>22.0</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="18">
+        <v>90.0</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47" s="18">
+        <v>4.6</v>
+      </c>
+      <c r="J47" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="K47" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L47" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M47" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N47" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="O47" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="P47" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="Q47" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="R47" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="S47" s="18">
+        <v>5.0</v>
+      </c>
+      <c r="T47" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="U47" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="V47" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="W47" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="X47" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Y47" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Z47" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="AA47" s="19">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="14">
+        <v>45742.44653422454</v>
+      </c>
+      <c r="B48" s="15">
+        <v>22.0</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="15">
+        <v>43.0</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="15">
+        <v>4.4</v>
+      </c>
+      <c r="J48" s="15">
+        <v>4.4</v>
+      </c>
+      <c r="K48" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L48" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M48" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="O48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="P48" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="Q48" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="R48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="S48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="T48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="U48" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="V48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="W48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="X48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="Y48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="Z48" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="AA48" s="16">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="17">
+        <v>45742.44900145833</v>
+      </c>
+      <c r="B49" s="18">
+        <v>22.0</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="18">
+        <v>86.25</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I49" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="J49" s="18">
+        <v>4.4</v>
+      </c>
+      <c r="K49" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M49" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N49" s="18">
+        <v>5.0</v>
+      </c>
+      <c r="O49" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="P49" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Q49" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="R49" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="S49" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="T49" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="U49" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="V49" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="W49" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="X49" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Y49" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="Z49" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="AA49" s="19">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="14">
+        <v>45742.45014104167</v>
+      </c>
+      <c r="B50" s="15">
+        <v>21.0</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="15">
+        <v>85.0</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" s="15">
+        <v>4.62</v>
+      </c>
+      <c r="J50" s="15">
+        <v>4.54</v>
+      </c>
+      <c r="K50" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L50" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M50" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N50" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="O50" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="P50" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="Q50" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="R50" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="S50" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="T50" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="U50" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="V50" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="W50" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="X50" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="Y50" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="Z50" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="AA50" s="16">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="17">
+        <v>45742.451680474536</v>
+      </c>
+      <c r="B51" s="18">
+        <v>24.0</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="18">
+        <v>90.0</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51" s="18">
+        <v>4.76</v>
+      </c>
+      <c r="J51" s="18">
+        <v>4.68</v>
+      </c>
+      <c r="K51" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L51" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="M51" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N51" s="18">
+        <v>5.0</v>
+      </c>
+      <c r="O51" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="P51" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="Q51" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="R51" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="S51" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="T51" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="U51" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="V51" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="W51" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="X51" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="Y51" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="Z51" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="AA51" s="19">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="14">
+        <v>45742.45519474537</v>
+      </c>
+      <c r="B52" s="15">
+        <v>24.0</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="15">
+        <v>3.969</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I52" s="15">
+        <v>3.59</v>
+      </c>
+      <c r="J52" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="K52" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L52" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M52" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N52" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="O52" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="P52" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="Q52" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="R52" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="S52" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="T52" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="U52" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="V52" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="W52" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="X52" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="Y52" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="Z52" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="AA52" s="16">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="24">
+        <v>45742.460507800926</v>
+      </c>
+      <c r="B53" s="25">
+        <v>22.0</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="25">
+        <v>86.625</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F53" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I53" s="25">
+        <v>4.33</v>
+      </c>
+      <c r="J53" s="25">
+        <v>4.7</v>
+      </c>
+      <c r="K53" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L53" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="M53" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N53" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="O53" s="25">
+        <v>4.0</v>
+      </c>
+      <c r="P53" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="Q53" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="R53" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="S53" s="25">
+        <v>4.0</v>
+      </c>
+      <c r="T53" s="25">
+        <v>5.0</v>
+      </c>
+      <c r="U53" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="V53" s="25">
+        <v>4.0</v>
+      </c>
+      <c r="W53" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="X53" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="Y53" s="25">
+        <v>4.0</v>
+      </c>
+      <c r="Z53" s="25">
+        <v>4.0</v>
+      </c>
+      <c r="AA53" s="26">
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>